<commit_message>
decode NWGL signal names
</commit_message>
<xml_diff>
--- a/EC/Train Runs and Enforcements 2016-06-29.xlsx
+++ b/EC/Train Runs and Enforcements 2016-06-29.xlsx
@@ -2098,10 +2098,10 @@
     <t>Onboard comparator issue caused comm outage</t>
   </si>
   <si>
-    <t>Premature downgrade at signal RTDC:00:00000300:00000012:00003293</t>
-  </si>
-  <si>
-    <t>Inefficient dispatching at RTDC:00:00000300:00000015:00000197</t>
+    <t>Premature downgrade at NW0109XH (BNSF FUEL CROSSING) 11-1T 1S</t>
+  </si>
+  <si>
+    <t>Inefficient dispatching at NW0137RH (38TH &amp; 41ST AVE) Signal 6S</t>
   </si>
 </sst>
 </file>
@@ -2628,24 +2628,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2687,20 +2669,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2723,46 +2693,42 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_XINGS" xfId="1"/>
   </cellStyles>
-  <dxfs count="44">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -2803,14 +2769,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2831,7 +2790,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2890,186 +2856,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3382,19 +3168,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="91" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="85" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="51" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" style="51" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" style="51" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" style="84" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" style="84" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" style="85" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" style="84" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" style="84" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="78" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" style="78" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="79" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" style="78" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" style="78" customWidth="1"/>
     <col min="10" max="10" width="7.7109375" style="51" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="13.28515625" style="51" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" style="92" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="93" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" style="86" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="87" customWidth="1"/>
     <col min="15" max="15" width="9.140625" style="2"/>
     <col min="16" max="16" width="6" style="2" customWidth="1"/>
     <col min="17" max="17" width="13.5703125" customWidth="1"/>
@@ -3411,20 +3197,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:91" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="91"/>
+      <c r="A1" s="85"/>
       <c r="B1" s="51"/>
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
       <c r="J1" s="51"/>
       <c r="K1" s="51"/>
       <c r="L1" s="51"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="93"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="87"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="V1" s="31"/>
@@ -3437,26 +3223,26 @@
       <c r="AC1" s="32"/>
     </row>
     <row r="2" spans="1:91" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="91"/>
+      <c r="A2" s="85"/>
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
       <c r="D2" s="51"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="94">
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="97">
         <f>Variables!A2</f>
         <v>42550</v>
       </c>
-      <c r="J2" s="95"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="74" t="s">
+      <c r="J2" s="98"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="75"/>
-      <c r="O2" s="76"/>
+      <c r="N2" s="100"/>
+      <c r="O2" s="101"/>
       <c r="P2" s="2"/>
       <c r="V2" s="31"/>
       <c r="W2" s="31"/>
@@ -3468,24 +3254,24 @@
       <c r="AC2" s="32"/>
     </row>
     <row r="3" spans="1:91" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="91"/>
+      <c r="A3" s="85"/>
       <c r="B3" s="51"/>
       <c r="C3" s="51"/>
       <c r="D3" s="51"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="97" t="s">
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="98"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="100" t="s">
+      <c r="J3" s="103"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="101" t="s">
+      <c r="N3" s="91" t="s">
         <v>12</v>
       </c>
       <c r="O3" s="3" t="s">
@@ -3502,27 +3288,27 @@
       <c r="AC3" s="32"/>
     </row>
     <row r="4" spans="1:91" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="91"/>
+      <c r="A4" s="85"/>
       <c r="B4" s="51"/>
       <c r="C4" s="51"/>
       <c r="D4" s="51"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="86" t="s">
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="102">
+      <c r="J4" s="92">
         <f>COUNT($N$13:$P$1857)</f>
         <v>143</v>
       </c>
-      <c r="K4" s="102"/>
-      <c r="L4" s="102"/>
-      <c r="M4" s="103" t="s">
+      <c r="K4" s="92"/>
+      <c r="L4" s="92"/>
+      <c r="M4" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="N4" s="101" t="s">
+      <c r="N4" s="91" t="s">
         <v>15</v>
       </c>
       <c r="O4" s="3" t="s">
@@ -3539,28 +3325,28 @@
       <c r="AC4" s="32"/>
     </row>
     <row r="5" spans="1:91" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="91"/>
+      <c r="A5" s="85"/>
       <c r="B5" s="51"/>
       <c r="C5" s="51"/>
       <c r="D5" s="51"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="86" t="s">
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="102">
+      <c r="J5" s="92">
         <f>COUNT($N$13:$N$1857)</f>
         <v>131</v>
       </c>
-      <c r="K5" s="102"/>
-      <c r="L5" s="102"/>
-      <c r="M5" s="103">
+      <c r="K5" s="92"/>
+      <c r="L5" s="92"/>
+      <c r="M5" s="93">
         <f>AVERAGE($N$13:$N$857)</f>
         <v>69.240966920673358</v>
       </c>
-      <c r="N5" s="101">
+      <c r="N5" s="91">
         <f>MIN($N$13:$N$857)</f>
         <v>36.149999995250255</v>
       </c>
@@ -3579,28 +3365,28 @@
       <c r="AC5" s="32"/>
     </row>
     <row r="6" spans="1:91" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="91"/>
+      <c r="A6" s="85"/>
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
       <c r="D6" s="51"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="87" t="s">
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="78"/>
+      <c r="I6" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="102">
+      <c r="J6" s="92">
         <f>COUNT($O$13:$O$857)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="102"/>
-      <c r="L6" s="102"/>
-      <c r="M6" s="103">
+      <c r="K6" s="92"/>
+      <c r="L6" s="92"/>
+      <c r="M6" s="93">
         <f>IFERROR(AVERAGE($O$13:$O$857),0)</f>
         <v>0</v>
       </c>
-      <c r="N6" s="101">
+      <c r="N6" s="91">
         <f>MIN($O$13:$O$857)</f>
         <v>0</v>
       </c>
@@ -3619,27 +3405,27 @@
       <c r="AC6" s="32"/>
     </row>
     <row r="7" spans="1:91" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="91"/>
+      <c r="A7" s="85"/>
       <c r="B7" s="51"/>
       <c r="C7" s="51"/>
       <c r="D7" s="51"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="88" t="s">
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="78"/>
+      <c r="I7" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="102">
+      <c r="J7" s="92">
         <f>COUNT($P$13:$P$857)</f>
         <v>12</v>
       </c>
-      <c r="K7" s="102"/>
-      <c r="L7" s="102"/>
-      <c r="M7" s="103" t="s">
+      <c r="K7" s="92"/>
+      <c r="L7" s="92"/>
+      <c r="M7" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="101" t="s">
+      <c r="N7" s="91" t="s">
         <v>15</v>
       </c>
       <c r="O7" s="3" t="s">
@@ -3656,28 +3442,28 @@
       <c r="AC7" s="32"/>
     </row>
     <row r="8" spans="1:91" s="33" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="91"/>
+      <c r="A8" s="85"/>
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
       <c r="D8" s="51"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="86" t="s">
+      <c r="E8" s="78"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="78"/>
+      <c r="I8" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="102">
+      <c r="J8" s="92">
         <f>COUNT($N$13:$O$857)</f>
         <v>131</v>
       </c>
-      <c r="K8" s="102"/>
-      <c r="L8" s="102"/>
-      <c r="M8" s="103">
+      <c r="K8" s="92"/>
+      <c r="L8" s="92"/>
+      <c r="M8" s="93">
         <f>AVERAGE($N$13:$P$857)</f>
         <v>65.802214451791997</v>
       </c>
-      <c r="N8" s="101">
+      <c r="N8" s="91">
         <f>MIN($N$13:$O$857)</f>
         <v>36.149999995250255</v>
       </c>
@@ -3696,25 +3482,25 @@
       <c r="AC8" s="32"/>
     </row>
     <row r="9" spans="1:91" s="33" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="91"/>
+      <c r="A9" s="85"/>
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
       <c r="D9" s="51"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="86" t="s">
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="104">
+      <c r="J9" s="94">
         <f>J8/J4</f>
         <v>0.91608391608391604</v>
       </c>
-      <c r="K9" s="104"/>
-      <c r="L9" s="104"/>
-      <c r="M9" s="92"/>
-      <c r="N9" s="93"/>
+      <c r="K9" s="94"/>
+      <c r="L9" s="94"/>
+      <c r="M9" s="86"/>
+      <c r="N9" s="87"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="V9" s="31"/>
@@ -3727,20 +3513,20 @@
       <c r="AC9" s="32"/>
     </row>
     <row r="10" spans="1:91" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="91"/>
+      <c r="A10" s="85"/>
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
       <c r="D10" s="51"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="78"/>
       <c r="J10" s="51"/>
       <c r="K10" s="51"/>
       <c r="L10" s="51"/>
-      <c r="M10" s="92"/>
-      <c r="N10" s="93"/>
+      <c r="M10" s="86"/>
+      <c r="N10" s="87"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="V10" s="31"/>
@@ -3753,25 +3539,25 @@
       <c r="AC10" s="32"/>
     </row>
     <row r="11" spans="1:91" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="73" t="str">
+      <c r="A11" s="96" t="str">
         <f>"Eagle P3 System Performance - "&amp;TEXT(Variables!A2,"yyyy-mm-dd")</f>
         <v>Eagle P3 System Performance - 2016-06-29</v>
       </c>
-      <c r="B11" s="73"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="73"/>
-      <c r="N11" s="73"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="96"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="96"/>
+      <c r="H11" s="96"/>
+      <c r="I11" s="96"/>
+      <c r="J11" s="96"/>
+      <c r="K11" s="96"/>
+      <c r="L11" s="96"/>
+      <c r="M11" s="96"/>
+      <c r="N11" s="96"/>
+      <c r="O11" s="96"/>
+      <c r="P11" s="96"/>
     </row>
     <row r="12" spans="1:91" s="5" customFormat="1" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
@@ -6427,7 +6213,7 @@
       </c>
     </row>
     <row r="39" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="105" t="s">
+      <c r="A39" s="95" t="s">
         <v>269</v>
       </c>
       <c r="B39" s="34">
@@ -8060,7 +7846,7 @@
       </c>
     </row>
     <row r="56" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="105" t="s">
+      <c r="A56" s="95" t="s">
         <v>647</v>
       </c>
       <c r="B56" s="34">
@@ -8926,7 +8712,7 @@
       </c>
     </row>
     <row r="65" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="105" t="s">
+      <c r="A65" s="95" t="s">
         <v>547</v>
       </c>
       <c r="B65" s="34">
@@ -9982,7 +9768,7 @@
       </c>
     </row>
     <row r="76" spans="1:29" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="105" t="s">
+      <c r="A76" s="95" t="s">
         <v>294</v>
       </c>
       <c r="B76" s="34">
@@ -10227,11 +10013,11 @@
       <c r="Q78" s="35"/>
       <c r="R78" s="35"/>
       <c r="S78" s="59">
-        <f t="shared" ref="S78:S141" si="23">SUM(U78:U78)/12</f>
+        <f t="shared" ref="S78:S135" si="23">SUM(U78:U78)/12</f>
         <v>1</v>
       </c>
       <c r="T78" s="1" t="str">
-        <f t="shared" ref="T78:T141" si="24">IF(ISEVEN(LEFT(A78,3)),"Southbound","NorthBound")</f>
+        <f t="shared" ref="T78:T135" si="24">IF(ISEVEN(LEFT(A78,3)),"Southbound","NorthBound")</f>
         <v>NorthBound</v>
       </c>
       <c r="U78" s="1">
@@ -10239,11 +10025,11 @@
         <v>12</v>
       </c>
       <c r="V78" s="38" t="str">
-        <f t="shared" ref="V78:V141" si="25">"https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'"&amp;TEXT(E78-1/24/60,"yyyy-MM-DD hh:mm:ss")&amp;"-0600',mode:absolute,to:'"&amp;TEXT(I78+1/24/60,"yyyy-MM-DD hh:mm:ss")&amp;"-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed',"&amp;"'Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:"&amp;"(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc."&amp;B78&amp;"%22')),sort:!(Time,asc))"</f>
+        <f t="shared" ref="V78:V135" si="25">"https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'"&amp;TEXT(E78-1/24/60,"yyyy-MM-DD hh:mm:ss")&amp;"-0600',mode:absolute,to:'"&amp;TEXT(I78+1/24/60,"yyyy-MM-DD hh:mm:ss")&amp;"-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed',"&amp;"'Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:"&amp;"(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc."&amp;B78&amp;"%22')),sort:!(Time,asc))"</f>
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 11:40:10-0600',mode:absolute,to:'2016-06-29 12:27:25-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4044%22')),sort:!(Time,asc))</v>
       </c>
       <c r="W78" s="38" t="str">
-        <f t="shared" ref="W78:W141" si="26">IF(AA78&lt;23,"Y","N")</f>
+        <f t="shared" ref="W78:W135" si="26">IF(AA78&lt;23,"Y","N")</f>
         <v>N</v>
       </c>
       <c r="X78" s="38">
@@ -10251,15 +10037,15 @@
         <v>1</v>
       </c>
       <c r="Y78" s="38">
-        <f t="shared" ref="Y78:Y141" si="27">RIGHT(D78,LEN(D78)-4)/10000</f>
+        <f t="shared" ref="Y78:Y135" si="27">RIGHT(D78,LEN(D78)-4)/10000</f>
         <v>4.4900000000000002E-2</v>
       </c>
       <c r="Z78" s="38">
-        <f t="shared" ref="Z78:Z141" si="28">RIGHT(H78,LEN(H78)-4)/10000</f>
+        <f t="shared" ref="Z78:Z135" si="28">RIGHT(H78,LEN(H78)-4)/10000</f>
         <v>23.331199999999999</v>
       </c>
       <c r="AA78" s="38">
-        <f t="shared" ref="AA78:AA141" si="29">ABS(Z78-Y78)</f>
+        <f t="shared" ref="AA78:AA135" si="29">ABS(Z78-Y78)</f>
         <v>23.286300000000001</v>
       </c>
       <c r="AB78" s="39" t="e">
@@ -10343,7 +10129,7 @@
         <v>N</v>
       </c>
       <c r="X79" s="38">
-        <f t="shared" ref="X78:X141" si="30">VALUE(LEFT(A79,3))-VALUE(LEFT(A78,3))</f>
+        <f t="shared" ref="X79:X135" si="30">VALUE(LEFT(A79,3))-VALUE(LEFT(A78,3))</f>
         <v>2</v>
       </c>
       <c r="Y79" s="38">
@@ -17578,19 +17364,19 @@
       <c r="D155" s="72" t="s">
         <v>288</v>
       </c>
-      <c r="E155" s="89">
+      <c r="E155" s="83">
         <v>42551.015069444446</v>
       </c>
-      <c r="F155" s="89">
+      <c r="F155" s="83">
         <v>42551.016111111108</v>
       </c>
-      <c r="G155" s="90">
-        <v>1</v>
-      </c>
-      <c r="H155" s="89" t="s">
+      <c r="G155" s="84">
+        <v>1</v>
+      </c>
+      <c r="H155" s="83" t="s">
         <v>96</v>
       </c>
-      <c r="I155" s="89">
+      <c r="I155" s="83">
         <v>42551.046979166669</v>
       </c>
       <c r="J155" s="72">
@@ -17772,19 +17558,19 @@
       <c r="D157" s="72" t="s">
         <v>201</v>
       </c>
-      <c r="E157" s="89">
+      <c r="E157" s="83">
         <v>42551.037962962961</v>
       </c>
-      <c r="F157" s="89">
+      <c r="F157" s="83">
         <v>42551.039236111108</v>
       </c>
-      <c r="G157" s="90">
-        <v>1</v>
-      </c>
-      <c r="H157" s="89" t="s">
+      <c r="G157" s="84">
+        <v>1</v>
+      </c>
+      <c r="H157" s="83" t="s">
         <v>75</v>
       </c>
-      <c r="I157" s="89">
+      <c r="I157" s="83">
         <v>42551.065011574072</v>
       </c>
       <c r="J157" s="72">
@@ -17868,19 +17654,19 @@
       <c r="D158" s="72" t="s">
         <v>164</v>
       </c>
-      <c r="E158" s="89">
+      <c r="E158" s="83">
         <v>42551.016296296293</v>
       </c>
-      <c r="F158" s="89">
+      <c r="F158" s="83">
         <v>42551.017094907409</v>
       </c>
-      <c r="G158" s="90">
-        <v>1</v>
-      </c>
-      <c r="H158" s="89" t="s">
+      <c r="G158" s="84">
+        <v>1</v>
+      </c>
+      <c r="H158" s="83" t="s">
         <v>280</v>
       </c>
-      <c r="I158" s="89">
+      <c r="I158" s="83">
         <v>42551.046226851853</v>
       </c>
       <c r="J158" s="72">
@@ -17964,19 +17750,19 @@
       <c r="D159" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="E159" s="89">
+      <c r="E159" s="83">
         <v>42551.056157407409</v>
       </c>
-      <c r="F159" s="89">
+      <c r="F159" s="83">
         <v>42551.057071759256</v>
       </c>
-      <c r="G159" s="90">
-        <v>1</v>
-      </c>
-      <c r="H159" s="89" t="s">
+      <c r="G159" s="84">
+        <v>1</v>
+      </c>
+      <c r="H159" s="83" t="s">
         <v>166</v>
       </c>
-      <c r="I159" s="89">
+      <c r="I159" s="83">
         <v>42551.086076388892</v>
       </c>
       <c r="J159" s="72">
@@ -18048,7 +17834,7 @@
       </c>
     </row>
     <row r="160" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A160" s="91" t="s">
+      <c r="A160" s="85" t="s">
         <v>414</v>
       </c>
       <c r="B160" s="51">
@@ -18060,42 +17846,42 @@
       <c r="D160" s="51" t="s">
         <v>415</v>
       </c>
-      <c r="E160" s="84">
+      <c r="E160" s="78">
         <v>42550.217349537037</v>
       </c>
-      <c r="F160" s="84">
+      <c r="F160" s="78">
         <v>42550.218368055554</v>
       </c>
-      <c r="G160" s="85">
-        <v>1</v>
-      </c>
-      <c r="H160" s="84" t="s">
+      <c r="G160" s="79">
+        <v>1</v>
+      </c>
+      <c r="H160" s="78" t="s">
         <v>416</v>
       </c>
-      <c r="I160" s="84">
+      <c r="I160" s="78">
         <v>42550.234525462962</v>
       </c>
       <c r="J160" s="51">
         <v>0</v>
       </c>
-      <c r="K160" s="79" t="str">
+      <c r="K160" s="73" t="str">
         <f t="shared" si="44"/>
         <v>4029/4030</v>
       </c>
-      <c r="L160" s="79" t="str">
+      <c r="L160" s="73" t="str">
         <f>VLOOKUP(A160,'Trips&amp;Operators'!$C$1:$E$10000,3,FALSE)</f>
         <v>STURGEON</v>
       </c>
-      <c r="M160" s="80">
+      <c r="M160" s="74">
         <f t="shared" si="45"/>
         <v>1.615740740817273E-2</v>
       </c>
-      <c r="N160" s="81"/>
-      <c r="O160" s="81"/>
-      <c r="P160" s="81"/>
-      <c r="Q160" s="82"/>
-      <c r="R160" s="82"/>
-      <c r="S160" s="83"/>
+      <c r="N160" s="75"/>
+      <c r="O160" s="75"/>
+      <c r="P160" s="75"/>
+      <c r="Q160" s="76"/>
+      <c r="R160" s="76"/>
+      <c r="S160" s="77"/>
       <c r="T160" s="1"/>
       <c r="U160" s="1"/>
       <c r="V160" s="38"/>
@@ -18108,7 +17894,7 @@
       <c r="AC160" s="39"/>
     </row>
     <row r="161" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A161" s="91" t="s">
+      <c r="A161" s="85" t="s">
         <v>417</v>
       </c>
       <c r="B161" s="51">
@@ -18120,19 +17906,19 @@
       <c r="D161" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="E161" s="84">
+      <c r="E161" s="78">
         <v>42550.236215277779</v>
       </c>
-      <c r="F161" s="84">
+      <c r="F161" s="78">
         <v>42550.237847222219</v>
       </c>
-      <c r="G161" s="85">
+      <c r="G161" s="79">
         <v>2</v>
       </c>
-      <c r="H161" s="84" t="s">
+      <c r="H161" s="78" t="s">
         <v>418</v>
       </c>
-      <c r="I161" s="84">
+      <c r="I161" s="78">
         <v>42550.256539351853</v>
       </c>
       <c r="J161" s="51">
@@ -18168,7 +17954,7 @@
       <c r="AC161" s="39"/>
     </row>
     <row r="162" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A162" s="91" t="s">
+      <c r="A162" s="85" t="s">
         <v>419</v>
       </c>
       <c r="B162" s="51">
@@ -18180,19 +17966,19 @@
       <c r="D162" s="51" t="s">
         <v>420</v>
       </c>
-      <c r="E162" s="84">
+      <c r="E162" s="78">
         <v>42550.2577662037</v>
       </c>
-      <c r="F162" s="84">
+      <c r="F162" s="78">
         <v>42550.258715277778</v>
       </c>
-      <c r="G162" s="85">
-        <v>1</v>
-      </c>
-      <c r="H162" s="84" t="s">
+      <c r="G162" s="79">
+        <v>1</v>
+      </c>
+      <c r="H162" s="78" t="s">
         <v>421</v>
       </c>
-      <c r="I162" s="84">
+      <c r="I162" s="78">
         <v>42550.277685185189</v>
       </c>
       <c r="J162" s="51">
@@ -18228,7 +18014,7 @@
       <c r="AC162" s="39"/>
     </row>
     <row r="163" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A163" s="91" t="s">
+      <c r="A163" s="85" t="s">
         <v>422</v>
       </c>
       <c r="B163" s="51">
@@ -18240,19 +18026,19 @@
       <c r="D163" s="51" t="s">
         <v>423</v>
       </c>
-      <c r="E163" s="84">
+      <c r="E163" s="78">
         <v>42550.264513888891</v>
       </c>
-      <c r="F163" s="84">
+      <c r="F163" s="78">
         <v>42550.266226851854</v>
       </c>
-      <c r="G163" s="85">
+      <c r="G163" s="79">
         <v>2</v>
       </c>
-      <c r="H163" s="84" t="s">
+      <c r="H163" s="78" t="s">
         <v>424</v>
       </c>
-      <c r="I163" s="84">
+      <c r="I163" s="78">
         <v>42550.277627314812</v>
       </c>
       <c r="J163" s="51">
@@ -18288,7 +18074,7 @@
       <c r="AC163" s="39"/>
     </row>
     <row r="164" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A164" s="91" t="s">
+      <c r="A164" s="85" t="s">
         <v>425</v>
       </c>
       <c r="B164" s="51">
@@ -18300,19 +18086,19 @@
       <c r="D164" s="51" t="s">
         <v>426</v>
       </c>
-      <c r="E164" s="84">
+      <c r="E164" s="78">
         <v>42550.278344907405</v>
       </c>
-      <c r="F164" s="84">
+      <c r="F164" s="78">
         <v>42550.279895833337</v>
       </c>
-      <c r="G164" s="85">
+      <c r="G164" s="79">
         <v>2</v>
       </c>
-      <c r="H164" s="84" t="s">
+      <c r="H164" s="78" t="s">
         <v>427</v>
       </c>
-      <c r="I164" s="84">
+      <c r="I164" s="78">
         <v>42550.296331018515</v>
       </c>
       <c r="J164" s="51">
@@ -18348,7 +18134,7 @@
       <c r="AC164" s="39"/>
     </row>
     <row r="165" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A165" s="91" t="s">
+      <c r="A165" s="85" t="s">
         <v>428</v>
       </c>
       <c r="B165" s="51">
@@ -18360,19 +18146,19 @@
       <c r="D165" s="51" t="s">
         <v>429</v>
       </c>
-      <c r="E165" s="84">
+      <c r="E165" s="78">
         <v>42550.280428240738</v>
       </c>
-      <c r="F165" s="84">
+      <c r="F165" s="78">
         <v>42550.281261574077</v>
       </c>
-      <c r="G165" s="85">
-        <v>1</v>
-      </c>
-      <c r="H165" s="84" t="s">
+      <c r="G165" s="79">
+        <v>1</v>
+      </c>
+      <c r="H165" s="78" t="s">
         <v>430</v>
       </c>
-      <c r="I165" s="84">
+      <c r="I165" s="78">
         <v>42550.297002314815</v>
       </c>
       <c r="J165" s="51">
@@ -18408,7 +18194,7 @@
       <c r="AC165" s="39"/>
     </row>
     <row r="166" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A166" s="91" t="s">
+      <c r="A166" s="85" t="s">
         <v>431</v>
       </c>
       <c r="B166" s="51">
@@ -18420,19 +18206,19 @@
       <c r="D166" s="51" t="s">
         <v>432</v>
       </c>
-      <c r="E166" s="84">
+      <c r="E166" s="78">
         <v>42550.298321759263</v>
       </c>
-      <c r="F166" s="84">
+      <c r="F166" s="78">
         <v>42550.299224537041</v>
       </c>
-      <c r="G166" s="85">
-        <v>1</v>
-      </c>
-      <c r="H166" s="84" t="s">
+      <c r="G166" s="79">
+        <v>1</v>
+      </c>
+      <c r="H166" s="78" t="s">
         <v>433</v>
       </c>
-      <c r="I166" s="84">
+      <c r="I166" s="78">
         <v>42550.315833333334</v>
       </c>
       <c r="J166" s="51">
@@ -18468,7 +18254,7 @@
       <c r="AC166" s="39"/>
     </row>
     <row r="167" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A167" s="91" t="s">
+      <c r="A167" s="85" t="s">
         <v>434</v>
       </c>
       <c r="B167" s="51">
@@ -18480,19 +18266,19 @@
       <c r="D167" s="51" t="s">
         <v>435</v>
       </c>
-      <c r="E167" s="84">
+      <c r="E167" s="78">
         <v>42550.297638888886</v>
       </c>
-      <c r="F167" s="84">
+      <c r="F167" s="78">
         <v>42550.298888888887</v>
       </c>
-      <c r="G167" s="85">
-        <v>1</v>
-      </c>
-      <c r="H167" s="84" t="s">
+      <c r="G167" s="79">
+        <v>1</v>
+      </c>
+      <c r="H167" s="78" t="s">
         <v>436</v>
       </c>
-      <c r="I167" s="84">
+      <c r="I167" s="78">
         <v>42550.315682870372</v>
       </c>
       <c r="J167" s="51">
@@ -18528,7 +18314,7 @@
       <c r="AC167" s="39"/>
     </row>
     <row r="168" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A168" s="91" t="s">
+      <c r="A168" s="85" t="s">
         <v>437</v>
       </c>
       <c r="B168" s="51">
@@ -18540,19 +18326,19 @@
       <c r="D168" s="51" t="s">
         <v>438</v>
       </c>
-      <c r="E168" s="84">
+      <c r="E168" s="78">
         <v>42550.31659722222</v>
       </c>
-      <c r="F168" s="84">
+      <c r="F168" s="78">
         <v>42550.317708333336</v>
       </c>
-      <c r="G168" s="85">
-        <v>1</v>
-      </c>
-      <c r="H168" s="84" t="s">
+      <c r="G168" s="79">
+        <v>1</v>
+      </c>
+      <c r="H168" s="78" t="s">
         <v>439</v>
       </c>
-      <c r="I168" s="84">
+      <c r="I168" s="78">
         <v>42550.33699074074</v>
       </c>
       <c r="J168" s="51">
@@ -18588,7 +18374,7 @@
       <c r="AC168" s="39"/>
     </row>
     <row r="169" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A169" s="91" t="s">
+      <c r="A169" s="85" t="s">
         <v>440</v>
       </c>
       <c r="B169" s="51">
@@ -18600,19 +18386,19 @@
       <c r="D169" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="E169" s="84">
+      <c r="E169" s="78">
         <v>42550.323981481481</v>
       </c>
-      <c r="F169" s="84">
+      <c r="F169" s="78">
         <v>42550.324780092589</v>
       </c>
-      <c r="G169" s="85">
-        <v>1</v>
-      </c>
-      <c r="H169" s="84" t="s">
+      <c r="G169" s="79">
+        <v>1</v>
+      </c>
+      <c r="H169" s="78" t="s">
         <v>441</v>
       </c>
-      <c r="I169" s="84">
+      <c r="I169" s="78">
         <v>42550.33798611111</v>
       </c>
       <c r="J169" s="51">
@@ -18648,7 +18434,7 @@
       <c r="AC169" s="39"/>
     </row>
     <row r="170" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A170" s="91" t="s">
+      <c r="A170" s="85" t="s">
         <v>442</v>
       </c>
       <c r="B170" s="51">
@@ -18660,19 +18446,19 @@
       <c r="D170" s="51" t="s">
         <v>443</v>
       </c>
-      <c r="E170" s="84">
+      <c r="E170" s="78">
         <v>42550.339201388888</v>
       </c>
-      <c r="F170" s="84">
+      <c r="F170" s="78">
         <v>42550.340150462966</v>
       </c>
-      <c r="G170" s="85">
-        <v>1</v>
-      </c>
-      <c r="H170" s="84" t="s">
+      <c r="G170" s="79">
+        <v>1</v>
+      </c>
+      <c r="H170" s="78" t="s">
         <v>444</v>
       </c>
-      <c r="I170" s="84">
+      <c r="I170" s="78">
         <v>42550.355509259258</v>
       </c>
       <c r="J170" s="51">
@@ -18708,7 +18494,7 @@
       <c r="AC170" s="39"/>
     </row>
     <row r="171" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A171" s="91" t="s">
+      <c r="A171" s="85" t="s">
         <v>600</v>
       </c>
       <c r="B171" s="51">
@@ -18720,19 +18506,19 @@
       <c r="D171" s="51" t="s">
         <v>659</v>
       </c>
-      <c r="E171" s="84">
+      <c r="E171" s="78">
         <v>42550.347037037034</v>
       </c>
-      <c r="F171" s="84">
+      <c r="F171" s="78">
         <v>42550.349305555559</v>
       </c>
-      <c r="G171" s="85">
+      <c r="G171" s="79">
         <v>3</v>
       </c>
-      <c r="H171" s="84" t="s">
+      <c r="H171" s="78" t="s">
         <v>660</v>
       </c>
-      <c r="I171" s="84">
+      <c r="I171" s="78">
         <v>42550.358657407407</v>
       </c>
       <c r="J171" s="51">
@@ -18768,7 +18554,7 @@
       <c r="AC171" s="39"/>
     </row>
     <row r="172" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A172" s="91" t="s">
+      <c r="A172" s="85" t="s">
         <v>528</v>
       </c>
       <c r="B172" s="51">
@@ -18780,19 +18566,19 @@
       <c r="D172" s="51" t="s">
         <v>661</v>
       </c>
-      <c r="E172" s="84">
+      <c r="E172" s="78">
         <v>42550.359467592592</v>
       </c>
-      <c r="F172" s="84">
+      <c r="F172" s="78">
         <v>42550.361550925925</v>
       </c>
-      <c r="G172" s="85">
+      <c r="G172" s="79">
         <v>2</v>
       </c>
-      <c r="H172" s="84" t="s">
+      <c r="H172" s="78" t="s">
         <v>662</v>
       </c>
-      <c r="I172" s="84">
+      <c r="I172" s="78">
         <v>42550.372870370367</v>
       </c>
       <c r="J172" s="51">
@@ -18828,7 +18614,7 @@
       <c r="AC172" s="39"/>
     </row>
     <row r="173" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A173" s="91" t="s">
+      <c r="A173" s="85" t="s">
         <v>529</v>
       </c>
       <c r="B173" s="51">
@@ -18840,19 +18626,19 @@
       <c r="D173" s="51" t="s">
         <v>663</v>
       </c>
-      <c r="E173" s="84">
+      <c r="E173" s="78">
         <v>42550.383634259262</v>
       </c>
-      <c r="F173" s="84">
+      <c r="F173" s="78">
         <v>42550.384571759256</v>
       </c>
-      <c r="G173" s="85">
-        <v>1</v>
-      </c>
-      <c r="H173" s="84" t="s">
+      <c r="G173" s="79">
+        <v>1</v>
+      </c>
+      <c r="H173" s="78" t="s">
         <v>441</v>
       </c>
-      <c r="I173" s="84">
+      <c r="I173" s="78">
         <v>42550.399131944447</v>
       </c>
       <c r="J173" s="51">
@@ -18888,7 +18674,7 @@
       <c r="AC173" s="39"/>
     </row>
     <row r="174" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A174" s="91" t="s">
+      <c r="A174" s="85" t="s">
         <v>548</v>
       </c>
       <c r="B174" s="51">
@@ -18900,19 +18686,19 @@
       <c r="D174" s="51" t="s">
         <v>664</v>
       </c>
-      <c r="E174" s="84">
+      <c r="E174" s="78">
         <v>42550.399942129632</v>
       </c>
-      <c r="F174" s="84">
+      <c r="F174" s="78">
         <v>42550.40084490741</v>
       </c>
-      <c r="G174" s="85">
-        <v>1</v>
-      </c>
-      <c r="H174" s="84" t="s">
+      <c r="G174" s="79">
+        <v>1</v>
+      </c>
+      <c r="H174" s="78" t="s">
         <v>665</v>
       </c>
-      <c r="I174" s="84">
+      <c r="I174" s="78">
         <v>42550.412812499999</v>
       </c>
       <c r="J174" s="51">
@@ -18948,7 +18734,7 @@
       <c r="AC174" s="39"/>
     </row>
     <row r="175" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A175" s="91" t="s">
+      <c r="A175" s="85" t="s">
         <v>536</v>
       </c>
       <c r="B175" s="51">
@@ -18960,19 +18746,19 @@
       <c r="D175" s="51" t="s">
         <v>666</v>
       </c>
-      <c r="E175" s="84">
+      <c r="E175" s="78">
         <v>42550.415532407409</v>
       </c>
-      <c r="F175" s="84">
+      <c r="F175" s="78">
         <v>42550.416770833333</v>
       </c>
-      <c r="G175" s="85">
-        <v>1</v>
-      </c>
-      <c r="H175" s="84" t="s">
+      <c r="G175" s="79">
+        <v>1</v>
+      </c>
+      <c r="H175" s="78" t="s">
         <v>441</v>
       </c>
-      <c r="I175" s="84">
+      <c r="I175" s="78">
         <v>42550.441562499997</v>
       </c>
       <c r="J175" s="51">
@@ -19008,7 +18794,7 @@
       <c r="AC175" s="39"/>
     </row>
     <row r="176" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A176" s="91" t="s">
+      <c r="A176" s="85" t="s">
         <v>636</v>
       </c>
       <c r="B176" s="51">
@@ -19020,19 +18806,19 @@
       <c r="D176" s="51" t="s">
         <v>500</v>
       </c>
-      <c r="E176" s="84">
+      <c r="E176" s="78">
         <v>42550.442546296297</v>
       </c>
-      <c r="F176" s="84">
+      <c r="F176" s="78">
         <v>42550.443611111114</v>
       </c>
-      <c r="G176" s="85">
-        <v>1</v>
-      </c>
-      <c r="H176" s="84" t="s">
+      <c r="G176" s="79">
+        <v>1</v>
+      </c>
+      <c r="H176" s="78" t="s">
         <v>667</v>
       </c>
-      <c r="I176" s="84">
+      <c r="I176" s="78">
         <v>42550.455196759256</v>
       </c>
       <c r="J176" s="51">
@@ -19068,7 +18854,7 @@
       <c r="AC176" s="39"/>
     </row>
     <row r="177" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A177" s="91" t="s">
+      <c r="A177" s="85" t="s">
         <v>445</v>
       </c>
       <c r="B177" s="51">
@@ -19080,19 +18866,19 @@
       <c r="D177" s="51" t="s">
         <v>446</v>
       </c>
-      <c r="E177" s="84">
+      <c r="E177" s="78">
         <v>42550.456516203703</v>
       </c>
-      <c r="F177" s="84">
+      <c r="F177" s="78">
         <v>42550.457743055558</v>
       </c>
-      <c r="G177" s="85">
-        <v>1</v>
-      </c>
-      <c r="H177" s="84" t="s">
+      <c r="G177" s="79">
+        <v>1</v>
+      </c>
+      <c r="H177" s="78" t="s">
         <v>447</v>
       </c>
-      <c r="I177" s="84">
+      <c r="I177" s="78">
         <v>42550.482557870368</v>
       </c>
       <c r="J177" s="51">
@@ -19128,7 +18914,7 @@
       <c r="AC177" s="39"/>
     </row>
     <row r="178" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A178" s="91" t="s">
+      <c r="A178" s="85" t="s">
         <v>448</v>
       </c>
       <c r="B178" s="51">
@@ -19140,19 +18926,19 @@
       <c r="D178" s="51" t="s">
         <v>449</v>
       </c>
-      <c r="E178" s="84">
+      <c r="E178" s="78">
         <v>42550.483437499999</v>
       </c>
-      <c r="F178" s="84">
+      <c r="F178" s="78">
         <v>42550.484293981484</v>
       </c>
-      <c r="G178" s="85">
-        <v>1</v>
-      </c>
-      <c r="H178" s="84" t="s">
+      <c r="G178" s="79">
+        <v>1</v>
+      </c>
+      <c r="H178" s="78" t="s">
         <v>450</v>
       </c>
-      <c r="I178" s="84">
+      <c r="I178" s="78">
         <v>42550.49790509259</v>
       </c>
       <c r="J178" s="51">
@@ -19188,7 +18974,7 @@
       <c r="AC178" s="39"/>
     </row>
     <row r="179" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A179" s="91" t="s">
+      <c r="A179" s="85" t="s">
         <v>451</v>
       </c>
       <c r="B179" s="51">
@@ -19200,19 +18986,19 @@
       <c r="D179" s="51" t="s">
         <v>452</v>
       </c>
-      <c r="E179" s="84">
+      <c r="E179" s="78">
         <v>42550.499062499999</v>
       </c>
-      <c r="F179" s="84">
+      <c r="F179" s="78">
         <v>42550.500659722224</v>
       </c>
-      <c r="G179" s="85">
+      <c r="G179" s="79">
         <v>2</v>
       </c>
-      <c r="H179" s="84" t="s">
+      <c r="H179" s="78" t="s">
         <v>418</v>
       </c>
-      <c r="I179" s="84">
+      <c r="I179" s="78">
         <v>42550.524131944447</v>
       </c>
       <c r="J179" s="51">
@@ -19238,7 +19024,7 @@
       <c r="S179" s="59"/>
     </row>
     <row r="180" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A180" s="91" t="s">
+      <c r="A180" s="85" t="s">
         <v>453</v>
       </c>
       <c r="B180" s="51">
@@ -19250,19 +19036,19 @@
       <c r="D180" s="51" t="s">
         <v>454</v>
       </c>
-      <c r="E180" s="84">
+      <c r="E180" s="78">
         <v>42550.524918981479</v>
       </c>
-      <c r="F180" s="84">
+      <c r="F180" s="78">
         <v>42550.525902777779</v>
       </c>
-      <c r="G180" s="85">
-        <v>1</v>
-      </c>
-      <c r="H180" s="84" t="s">
+      <c r="G180" s="79">
+        <v>1</v>
+      </c>
+      <c r="H180" s="78" t="s">
         <v>455</v>
       </c>
-      <c r="I180" s="84">
+      <c r="I180" s="78">
         <v>42550.538599537038</v>
       </c>
       <c r="J180" s="51">
@@ -19288,7 +19074,7 @@
       <c r="S180" s="59"/>
     </row>
     <row r="181" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A181" s="91" t="s">
+      <c r="A181" s="85" t="s">
         <v>456</v>
       </c>
       <c r="B181" s="51">
@@ -19300,19 +19086,19 @@
       <c r="D181" s="51" t="s">
         <v>457</v>
       </c>
-      <c r="E181" s="84">
+      <c r="E181" s="78">
         <v>42550.540185185186</v>
       </c>
-      <c r="F181" s="84">
+      <c r="F181" s="78">
         <v>42550.541631944441</v>
       </c>
-      <c r="G181" s="85">
+      <c r="G181" s="79">
         <v>2</v>
       </c>
-      <c r="H181" s="84" t="s">
+      <c r="H181" s="78" t="s">
         <v>458</v>
       </c>
-      <c r="I181" s="84">
+      <c r="I181" s="78">
         <v>42550.566458333335</v>
       </c>
       <c r="J181" s="51">
@@ -19338,7 +19124,7 @@
       <c r="S181" s="59"/>
     </row>
     <row r="182" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A182" s="91" t="s">
+      <c r="A182" s="85" t="s">
         <v>459</v>
       </c>
       <c r="B182" s="51">
@@ -19350,19 +19136,19 @@
       <c r="D182" s="51" t="s">
         <v>460</v>
       </c>
-      <c r="E182" s="84">
+      <c r="E182" s="78">
         <v>42550.567129629628</v>
       </c>
-      <c r="F182" s="84">
+      <c r="F182" s="78">
         <v>42550.567997685182</v>
       </c>
-      <c r="G182" s="85">
-        <v>1</v>
-      </c>
-      <c r="H182" s="84" t="s">
+      <c r="G182" s="79">
+        <v>1</v>
+      </c>
+      <c r="H182" s="78" t="s">
         <v>461</v>
       </c>
-      <c r="I182" s="84">
+      <c r="I182" s="78">
         <v>42550.579664351855</v>
       </c>
       <c r="J182" s="51">
@@ -19388,7 +19174,7 @@
       <c r="S182" s="59"/>
     </row>
     <row r="183" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A183" s="91" t="s">
+      <c r="A183" s="85" t="s">
         <v>462</v>
       </c>
       <c r="B183" s="51">
@@ -19400,19 +19186,19 @@
       <c r="D183" s="51" t="s">
         <v>463</v>
       </c>
-      <c r="E183" s="84">
+      <c r="E183" s="78">
         <v>42550.592118055552</v>
       </c>
-      <c r="F183" s="84">
+      <c r="F183" s="78">
         <v>42550.632511574076</v>
       </c>
-      <c r="G183" s="85">
+      <c r="G183" s="79">
         <v>58</v>
       </c>
-      <c r="H183" s="84" t="s">
+      <c r="H183" s="78" t="s">
         <v>464</v>
       </c>
-      <c r="I183" s="84">
+      <c r="I183" s="78">
         <v>42550.648657407408</v>
       </c>
       <c r="J183" s="51">
@@ -19438,7 +19224,7 @@
       <c r="S183" s="59"/>
     </row>
     <row r="184" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A184" s="91" t="s">
+      <c r="A184" s="85" t="s">
         <v>462</v>
       </c>
       <c r="B184" s="51">
@@ -19450,19 +19236,19 @@
       <c r="D184" s="51" t="s">
         <v>465</v>
       </c>
-      <c r="E184" s="84">
+      <c r="E184" s="78">
         <v>42550.592118055552</v>
       </c>
-      <c r="F184" s="84">
+      <c r="F184" s="78">
         <v>42550.593101851853</v>
       </c>
-      <c r="G184" s="85">
-        <v>1</v>
-      </c>
-      <c r="H184" s="84" t="s">
+      <c r="G184" s="79">
+        <v>1</v>
+      </c>
+      <c r="H184" s="78" t="s">
         <v>466</v>
       </c>
-      <c r="I184" s="84">
+      <c r="I184" s="78">
         <v>42550.606585648151</v>
       </c>
       <c r="J184" s="51">
@@ -19488,7 +19274,7 @@
       <c r="S184" s="59"/>
     </row>
     <row r="185" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A185" s="91" t="s">
+      <c r="A185" s="85" t="s">
         <v>467</v>
       </c>
       <c r="B185" s="51">
@@ -19500,19 +19286,19 @@
       <c r="D185" s="51" t="s">
         <v>468</v>
       </c>
-      <c r="E185" s="84">
+      <c r="E185" s="78">
         <v>42550.607743055552</v>
       </c>
-      <c r="F185" s="84">
+      <c r="F185" s="78">
         <v>42550.608657407407</v>
       </c>
-      <c r="G185" s="85">
-        <v>1</v>
-      </c>
-      <c r="H185" s="84" t="s">
+      <c r="G185" s="79">
+        <v>1</v>
+      </c>
+      <c r="H185" s="78" t="s">
         <v>469</v>
       </c>
-      <c r="I185" s="84">
+      <c r="I185" s="78">
         <v>42550.620752314811</v>
       </c>
       <c r="J185" s="51">
@@ -19538,7 +19324,7 @@
       <c r="S185" s="59"/>
     </row>
     <row r="186" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A186" s="91" t="s">
+      <c r="A186" s="85" t="s">
         <v>470</v>
       </c>
       <c r="B186" s="51">
@@ -19550,19 +19336,19 @@
       <c r="D186" s="51" t="s">
         <v>471</v>
       </c>
-      <c r="E186" s="84">
+      <c r="E186" s="78">
         <v>42550.649513888886</v>
       </c>
-      <c r="F186" s="84">
+      <c r="F186" s="78">
         <v>42550.650358796294</v>
       </c>
-      <c r="G186" s="85">
-        <v>1</v>
-      </c>
-      <c r="H186" s="84" t="s">
+      <c r="G186" s="79">
+        <v>1</v>
+      </c>
+      <c r="H186" s="78" t="s">
         <v>472</v>
       </c>
-      <c r="I186" s="84">
+      <c r="I186" s="78">
         <v>42550.66300925926</v>
       </c>
       <c r="J186" s="51">
@@ -19588,7 +19374,7 @@
       <c r="S186" s="59"/>
     </row>
     <row r="187" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A187" s="91" t="s">
+      <c r="A187" s="85" t="s">
         <v>473</v>
       </c>
       <c r="B187" s="51">
@@ -19600,19 +19386,19 @@
       <c r="D187" s="51" t="s">
         <v>474</v>
       </c>
-      <c r="E187" s="84">
+      <c r="E187" s="78">
         <v>42550.653344907405</v>
       </c>
-      <c r="F187" s="84">
+      <c r="F187" s="78">
         <v>42550.654467592591</v>
       </c>
-      <c r="G187" s="85">
-        <v>1</v>
-      </c>
-      <c r="H187" s="84" t="s">
+      <c r="G187" s="79">
+        <v>1</v>
+      </c>
+      <c r="H187" s="78" t="s">
         <v>475</v>
       </c>
-      <c r="I187" s="84">
+      <c r="I187" s="78">
         <v>42550.669791666667</v>
       </c>
       <c r="J187" s="51">
@@ -19638,7 +19424,7 @@
       <c r="S187" s="59"/>
     </row>
     <row r="188" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A188" s="91" t="s">
+      <c r="A188" s="85" t="s">
         <v>476</v>
       </c>
       <c r="B188" s="51">
@@ -19650,19 +19436,19 @@
       <c r="D188" s="51" t="s">
         <v>432</v>
       </c>
-      <c r="E188" s="84">
+      <c r="E188" s="78">
         <v>42550.67083333333</v>
       </c>
-      <c r="F188" s="84">
+      <c r="F188" s="78">
         <v>42550.671979166669</v>
       </c>
-      <c r="G188" s="85">
-        <v>1</v>
-      </c>
-      <c r="H188" s="84" t="s">
+      <c r="G188" s="79">
+        <v>1</v>
+      </c>
+      <c r="H188" s="78" t="s">
         <v>75</v>
       </c>
-      <c r="I188" s="84">
+      <c r="I188" s="78">
         <v>42550.685243055559</v>
       </c>
       <c r="J188" s="51">
@@ -19688,7 +19474,7 @@
       <c r="S188" s="59"/>
     </row>
     <row r="189" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A189" s="91" t="s">
+      <c r="A189" s="85" t="s">
         <v>477</v>
       </c>
       <c r="B189" s="51">
@@ -19700,19 +19486,19 @@
       <c r="D189" s="51" t="s">
         <v>478</v>
       </c>
-      <c r="E189" s="84">
+      <c r="E189" s="78">
         <v>42550.676944444444</v>
       </c>
-      <c r="F189" s="84">
+      <c r="F189" s="78">
         <v>42550.678078703706</v>
       </c>
-      <c r="G189" s="85">
-        <v>1</v>
-      </c>
-      <c r="H189" s="84" t="s">
+      <c r="G189" s="79">
+        <v>1</v>
+      </c>
+      <c r="H189" s="78" t="s">
         <v>479</v>
       </c>
-      <c r="I189" s="84">
+      <c r="I189" s="78">
         <v>42550.689687500002</v>
       </c>
       <c r="J189" s="51">
@@ -19738,7 +19524,7 @@
       <c r="S189" s="59"/>
     </row>
     <row r="190" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A190" s="91" t="s">
+      <c r="A190" s="85" t="s">
         <v>480</v>
       </c>
       <c r="B190" s="51">
@@ -19750,19 +19536,19 @@
       <c r="D190" s="51" t="s">
         <v>471</v>
       </c>
-      <c r="E190" s="84">
+      <c r="E190" s="78">
         <v>42550.692499999997</v>
       </c>
-      <c r="F190" s="84">
+      <c r="F190" s="78">
         <v>42550.69358796296</v>
       </c>
-      <c r="G190" s="85">
-        <v>1</v>
-      </c>
-      <c r="H190" s="84" t="s">
+      <c r="G190" s="79">
+        <v>1</v>
+      </c>
+      <c r="H190" s="78" t="s">
         <v>481</v>
       </c>
-      <c r="I190" s="84">
+      <c r="I190" s="78">
         <v>42550.703969907408</v>
       </c>
       <c r="J190" s="51">
@@ -19788,7 +19574,7 @@
       <c r="S190" s="59"/>
     </row>
     <row r="191" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A191" s="91" t="s">
+      <c r="A191" s="85" t="s">
         <v>482</v>
       </c>
       <c r="B191" s="51">
@@ -19800,19 +19586,19 @@
       <c r="D191" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="E191" s="84">
+      <c r="E191" s="78">
         <v>42550.694571759261</v>
       </c>
-      <c r="F191" s="84">
+      <c r="F191" s="78">
         <v>42550.696296296293</v>
       </c>
-      <c r="G191" s="85">
+      <c r="G191" s="79">
         <v>2</v>
       </c>
-      <c r="H191" s="84" t="s">
+      <c r="H191" s="78" t="s">
         <v>483</v>
       </c>
-      <c r="I191" s="84">
+      <c r="I191" s="78">
         <v>42550.711631944447</v>
       </c>
       <c r="J191" s="51">
@@ -19838,7 +19624,7 @@
       <c r="S191" s="59"/>
     </row>
     <row r="192" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A192" s="91" t="s">
+      <c r="A192" s="85" t="s">
         <v>484</v>
       </c>
       <c r="B192" s="51">
@@ -19850,19 +19636,19 @@
       <c r="D192" s="51" t="s">
         <v>485</v>
       </c>
-      <c r="E192" s="84">
+      <c r="E192" s="78">
         <v>42550.712916666664</v>
       </c>
-      <c r="F192" s="84">
+      <c r="F192" s="78">
         <v>42550.713912037034</v>
       </c>
-      <c r="G192" s="85">
-        <v>1</v>
-      </c>
-      <c r="H192" s="84" t="s">
+      <c r="G192" s="79">
+        <v>1</v>
+      </c>
+      <c r="H192" s="78" t="s">
         <v>486</v>
       </c>
-      <c r="I192" s="84">
+      <c r="I192" s="78">
         <v>42550.726527777777</v>
       </c>
       <c r="J192" s="51">
@@ -19888,7 +19674,7 @@
       <c r="S192" s="59"/>
     </row>
     <row r="193" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A193" s="91" t="s">
+      <c r="A193" s="85" t="s">
         <v>487</v>
       </c>
       <c r="B193" s="51">
@@ -19900,19 +19686,19 @@
       <c r="D193" s="51" t="s">
         <v>488</v>
       </c>
-      <c r="E193" s="84">
+      <c r="E193" s="78">
         <v>42550.719039351854</v>
       </c>
-      <c r="F193" s="84">
+      <c r="F193" s="78">
         <v>42550.720439814817</v>
       </c>
-      <c r="G193" s="85">
+      <c r="G193" s="79">
         <v>2</v>
       </c>
-      <c r="H193" s="84" t="s">
+      <c r="H193" s="78" t="s">
         <v>489</v>
       </c>
-      <c r="I193" s="84">
+      <c r="I193" s="78">
         <v>42550.731527777774</v>
       </c>
       <c r="J193" s="51">
@@ -19938,7 +19724,7 @@
       <c r="S193" s="59"/>
     </row>
     <row r="194" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A194" s="91" t="s">
+      <c r="A194" s="85" t="s">
         <v>490</v>
       </c>
       <c r="B194" s="51">
@@ -19950,19 +19736,19 @@
       <c r="D194" s="51" t="s">
         <v>491</v>
       </c>
-      <c r="E194" s="84">
+      <c r="E194" s="78">
         <v>42550.73364583333</v>
       </c>
-      <c r="F194" s="84">
+      <c r="F194" s="78">
         <v>42550.7344212963</v>
       </c>
-      <c r="G194" s="85">
-        <v>1</v>
-      </c>
-      <c r="H194" s="84" t="s">
+      <c r="G194" s="79">
+        <v>1</v>
+      </c>
+      <c r="H194" s="78" t="s">
         <v>469</v>
       </c>
-      <c r="I194" s="84">
+      <c r="I194" s="78">
         <v>42550.745613425926</v>
       </c>
       <c r="J194" s="51">
@@ -19988,7 +19774,7 @@
       <c r="S194" s="59"/>
     </row>
     <row r="195" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A195" s="91" t="s">
+      <c r="A195" s="85" t="s">
         <v>492</v>
       </c>
       <c r="B195" s="51">
@@ -20000,19 +19786,19 @@
       <c r="D195" s="51" t="s">
         <v>493</v>
       </c>
-      <c r="E195" s="84">
+      <c r="E195" s="78">
         <v>42550.738807870373</v>
       </c>
-      <c r="F195" s="84">
+      <c r="F195" s="78">
         <v>42550.739733796298</v>
       </c>
-      <c r="G195" s="85">
-        <v>1</v>
-      </c>
-      <c r="H195" s="84" t="s">
+      <c r="G195" s="79">
+        <v>1</v>
+      </c>
+      <c r="H195" s="78" t="s">
         <v>464</v>
       </c>
-      <c r="I195" s="84">
+      <c r="I195" s="78">
         <v>42550.75267361111</v>
       </c>
       <c r="J195" s="51">
@@ -20038,7 +19824,7 @@
       <c r="S195" s="59"/>
     </row>
     <row r="196" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A196" s="91" t="s">
+      <c r="A196" s="85" t="s">
         <v>494</v>
       </c>
       <c r="B196" s="51">
@@ -20050,19 +19836,19 @@
       <c r="D196" s="51" t="s">
         <v>495</v>
       </c>
-      <c r="E196" s="84">
+      <c r="E196" s="78">
         <v>42550.753865740742</v>
       </c>
-      <c r="F196" s="84">
+      <c r="F196" s="78">
         <v>42550.75472222222</v>
       </c>
-      <c r="G196" s="85">
-        <v>1</v>
-      </c>
-      <c r="H196" s="84" t="s">
+      <c r="G196" s="79">
+        <v>1</v>
+      </c>
+      <c r="H196" s="78" t="s">
         <v>496</v>
       </c>
-      <c r="I196" s="84">
+      <c r="I196" s="78">
         <v>42550.767534722225</v>
       </c>
       <c r="J196" s="51">
@@ -20088,7 +19874,7 @@
       <c r="S196" s="59"/>
     </row>
     <row r="197" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A197" s="91" t="s">
+      <c r="A197" s="85" t="s">
         <v>497</v>
       </c>
       <c r="B197" s="51">
@@ -20100,19 +19886,19 @@
       <c r="D197" s="51" t="s">
         <v>498</v>
       </c>
-      <c r="E197" s="84">
+      <c r="E197" s="78">
         <v>42550.76226851852</v>
       </c>
-      <c r="F197" s="84">
+      <c r="F197" s="78">
         <v>42550.764120370368</v>
       </c>
-      <c r="G197" s="85">
+      <c r="G197" s="79">
         <v>2</v>
       </c>
-      <c r="H197" s="84" t="s">
+      <c r="H197" s="78" t="s">
         <v>475</v>
       </c>
-      <c r="I197" s="84">
+      <c r="I197" s="78">
         <v>42550.773553240739</v>
       </c>
       <c r="J197" s="51">
@@ -20138,7 +19924,7 @@
       <c r="S197" s="59"/>
     </row>
     <row r="198" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A198" s="91" t="s">
+      <c r="A198" s="85" t="s">
         <v>499</v>
       </c>
       <c r="B198" s="51">
@@ -20150,19 +19936,19 @@
       <c r="D198" s="51" t="s">
         <v>500</v>
       </c>
-      <c r="E198" s="84">
+      <c r="E198" s="78">
         <v>42550.77753472222</v>
       </c>
-      <c r="F198" s="84">
+      <c r="F198" s="78">
         <v>42550.778437499997</v>
       </c>
-      <c r="G198" s="85">
-        <v>1</v>
-      </c>
-      <c r="H198" s="84" t="s">
+      <c r="G198" s="79">
+        <v>1</v>
+      </c>
+      <c r="H198" s="78" t="s">
         <v>501</v>
       </c>
-      <c r="I198" s="84">
+      <c r="I198" s="78">
         <v>42550.788287037038</v>
       </c>
       <c r="J198" s="51">
@@ -20188,7 +19974,7 @@
       <c r="S198" s="59"/>
     </row>
     <row r="199" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A199" s="91" t="s">
+      <c r="A199" s="85" t="s">
         <v>502</v>
       </c>
       <c r="B199" s="51">
@@ -20200,19 +19986,19 @@
       <c r="D199" s="51" t="s">
         <v>503</v>
       </c>
-      <c r="E199" s="84">
+      <c r="E199" s="78">
         <v>42550.782418981478</v>
       </c>
-      <c r="F199" s="84">
+      <c r="F199" s="78">
         <v>42550.783310185187</v>
       </c>
-      <c r="G199" s="85">
-        <v>1</v>
-      </c>
-      <c r="H199" s="84" t="s">
+      <c r="G199" s="79">
+        <v>1</v>
+      </c>
+      <c r="H199" s="78" t="s">
         <v>504</v>
       </c>
-      <c r="I199" s="84">
+      <c r="I199" s="78">
         <v>42550.796134259261</v>
       </c>
       <c r="J199" s="51">
@@ -20238,7 +20024,7 @@
       <c r="S199" s="59"/>
     </row>
     <row r="200" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A200" s="91" t="s">
+      <c r="A200" s="85" t="s">
         <v>505</v>
       </c>
       <c r="B200" s="51">
@@ -20250,19 +20036,19 @@
       <c r="D200" s="51" t="s">
         <v>415</v>
       </c>
-      <c r="E200" s="84">
+      <c r="E200" s="78">
         <v>42550.817141203705</v>
       </c>
-      <c r="F200" s="84">
+      <c r="F200" s="78">
         <v>42550.817939814813</v>
       </c>
-      <c r="G200" s="85">
-        <v>1</v>
-      </c>
-      <c r="H200" s="84" t="s">
+      <c r="G200" s="79">
+        <v>1</v>
+      </c>
+      <c r="H200" s="78" t="s">
         <v>506</v>
       </c>
-      <c r="I200" s="84">
+      <c r="I200" s="78">
         <v>42550.829606481479</v>
       </c>
       <c r="J200" s="51">
@@ -20288,7 +20074,7 @@
       <c r="S200" s="59"/>
     </row>
     <row r="201" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A201" s="91" t="s">
+      <c r="A201" s="85" t="s">
         <v>507</v>
       </c>
       <c r="B201" s="51">
@@ -20300,19 +20086,19 @@
       <c r="D201" s="51" t="s">
         <v>508</v>
       </c>
-      <c r="E201" s="84">
+      <c r="E201" s="78">
         <v>42550.803032407406</v>
       </c>
-      <c r="F201" s="84">
+      <c r="F201" s="78">
         <v>42550.803842592592</v>
       </c>
-      <c r="G201" s="85">
-        <v>1</v>
-      </c>
-      <c r="H201" s="84" t="s">
+      <c r="G201" s="79">
+        <v>1</v>
+      </c>
+      <c r="H201" s="78" t="s">
         <v>509</v>
       </c>
-      <c r="I201" s="84">
+      <c r="I201" s="78">
         <v>42550.81527777778</v>
       </c>
       <c r="J201" s="51">
@@ -20338,7 +20124,7 @@
       <c r="S201" s="59"/>
     </row>
     <row r="202" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A202" s="91" t="s">
+      <c r="A202" s="85" t="s">
         <v>507</v>
       </c>
       <c r="B202" s="51">
@@ -20350,19 +20136,19 @@
       <c r="D202" s="51" t="s">
         <v>510</v>
       </c>
-      <c r="E202" s="84">
+      <c r="E202" s="78">
         <v>42550.803032407406</v>
       </c>
-      <c r="F202" s="84">
+      <c r="F202" s="78">
         <v>42550.806898148148</v>
       </c>
-      <c r="G202" s="85">
+      <c r="G202" s="79">
         <v>5</v>
       </c>
-      <c r="H202" s="84" t="s">
+      <c r="H202" s="78" t="s">
         <v>509</v>
       </c>
-      <c r="I202" s="84">
+      <c r="I202" s="78">
         <v>42550.81527777778</v>
       </c>
       <c r="J202" s="51">
@@ -20388,7 +20174,7 @@
       <c r="S202" s="59"/>
     </row>
     <row r="203" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A203" s="91" t="s">
+      <c r="A203" s="85" t="s">
         <v>511</v>
       </c>
       <c r="B203" s="51">
@@ -20400,19 +20186,19 @@
       <c r="D203" s="51" t="s">
         <v>512</v>
       </c>
-      <c r="E203" s="84">
+      <c r="E203" s="78">
         <v>42550.857928240737</v>
       </c>
-      <c r="F203" s="84">
+      <c r="F203" s="78">
         <v>42550.858796296299</v>
       </c>
-      <c r="G203" s="85">
-        <v>1</v>
-      </c>
-      <c r="H203" s="84" t="s">
+      <c r="G203" s="79">
+        <v>1</v>
+      </c>
+      <c r="H203" s="78" t="s">
         <v>513</v>
       </c>
-      <c r="I203" s="84">
+      <c r="I203" s="78">
         <v>42550.870555555557</v>
       </c>
       <c r="J203" s="51">
@@ -20438,7 +20224,7 @@
       <c r="S203" s="59"/>
     </row>
     <row r="204" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A204" s="91" t="s">
+      <c r="A204" s="85" t="s">
         <v>514</v>
       </c>
       <c r="B204" s="51">
@@ -20450,19 +20236,19 @@
       <c r="D204" s="51" t="s">
         <v>478</v>
       </c>
-      <c r="E204" s="84">
+      <c r="E204" s="78">
         <v>42550.843194444446</v>
       </c>
-      <c r="F204" s="84">
+      <c r="F204" s="78">
         <v>42550.844571759262</v>
       </c>
-      <c r="G204" s="85">
-        <v>1</v>
-      </c>
-      <c r="H204" s="84" t="s">
+      <c r="G204" s="79">
+        <v>1</v>
+      </c>
+      <c r="H204" s="78" t="s">
         <v>515</v>
       </c>
-      <c r="I204" s="84">
+      <c r="I204" s="78">
         <v>42550.857164351852</v>
       </c>
       <c r="J204" s="51">
@@ -20488,7 +20274,7 @@
       <c r="S204" s="59"/>
     </row>
     <row r="205" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A205" s="91" t="s">
+      <c r="A205" s="85" t="s">
         <v>516</v>
       </c>
       <c r="B205" s="51">
@@ -20500,19 +20286,19 @@
       <c r="D205" s="51" t="s">
         <v>517</v>
       </c>
-      <c r="E205" s="84">
+      <c r="E205" s="78">
         <v>42550.899652777778</v>
       </c>
-      <c r="F205" s="84">
+      <c r="F205" s="78">
         <v>42550.900648148148</v>
       </c>
-      <c r="G205" s="85">
-        <v>1</v>
-      </c>
-      <c r="H205" s="84" t="s">
+      <c r="G205" s="79">
+        <v>1</v>
+      </c>
+      <c r="H205" s="78" t="s">
         <v>518</v>
       </c>
-      <c r="I205" s="84">
+      <c r="I205" s="78">
         <v>42550.913738425923</v>
       </c>
       <c r="J205" s="51">
@@ -20538,7 +20324,7 @@
       <c r="S205" s="59"/>
     </row>
     <row r="206" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A206" s="91" t="s">
+      <c r="A206" s="85" t="s">
         <v>519</v>
       </c>
       <c r="B206" s="51">
@@ -20550,19 +20336,19 @@
       <c r="D206" s="51" t="s">
         <v>463</v>
       </c>
-      <c r="E206" s="84">
+      <c r="E206" s="78">
         <v>42550.886307870373</v>
       </c>
-      <c r="F206" s="84">
+      <c r="F206" s="78">
         <v>42550.887280092589</v>
       </c>
-      <c r="G206" s="85">
-        <v>1</v>
-      </c>
-      <c r="H206" s="84" t="s">
+      <c r="G206" s="79">
+        <v>1</v>
+      </c>
+      <c r="H206" s="78" t="s">
         <v>520</v>
       </c>
-      <c r="I206" s="84">
+      <c r="I206" s="78">
         <v>42550.898055555554</v>
       </c>
       <c r="J206" s="51">
@@ -20588,7 +20374,7 @@
       <c r="S206" s="59"/>
     </row>
     <row r="207" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A207" s="91" t="s">
+      <c r="A207" s="85" t="s">
         <v>521</v>
       </c>
       <c r="B207" s="51">
@@ -20600,19 +20386,19 @@
       <c r="D207" s="51" t="s">
         <v>522</v>
       </c>
-      <c r="E207" s="84">
+      <c r="E207" s="78">
         <v>42550.926689814813</v>
       </c>
-      <c r="F207" s="84">
+      <c r="F207" s="78">
         <v>42550.927569444444</v>
       </c>
-      <c r="G207" s="85">
-        <v>1</v>
-      </c>
-      <c r="H207" s="84" t="s">
+      <c r="G207" s="79">
+        <v>1</v>
+      </c>
+      <c r="H207" s="78" t="s">
         <v>523</v>
       </c>
-      <c r="I207" s="84">
+      <c r="I207" s="78">
         <v>42550.940335648149</v>
       </c>
       <c r="J207" s="51">
@@ -20638,7 +20424,7 @@
       <c r="S207" s="59"/>
     </row>
     <row r="208" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A208" s="91" t="s">
+      <c r="A208" s="85" t="s">
         <v>629</v>
       </c>
       <c r="B208" s="51">
@@ -20650,19 +20436,19 @@
       <c r="D208" s="51" t="s">
         <v>668</v>
       </c>
-      <c r="E208" s="84">
+      <c r="E208" s="78">
         <v>42550.356793981482</v>
       </c>
-      <c r="F208" s="84">
+      <c r="F208" s="78">
         <v>42550.357662037037</v>
       </c>
-      <c r="G208" s="85">
-        <v>1</v>
-      </c>
-      <c r="H208" s="84" t="s">
+      <c r="G208" s="79">
+        <v>1</v>
+      </c>
+      <c r="H208" s="78" t="s">
         <v>669</v>
       </c>
-      <c r="I208" s="84">
+      <c r="I208" s="78">
         <v>42550.363333333335</v>
       </c>
       <c r="J208" s="51">
@@ -20688,7 +20474,7 @@
       <c r="S208" s="59"/>
     </row>
     <row r="209" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A209" s="91" t="s">
+      <c r="A209" s="85" t="s">
         <v>524</v>
       </c>
       <c r="B209" s="51">
@@ -20700,19 +20486,19 @@
       <c r="D209" s="51" t="s">
         <v>415</v>
       </c>
-      <c r="E209" s="84">
+      <c r="E209" s="78">
         <v>42550.797152777777</v>
       </c>
-      <c r="F209" s="84">
+      <c r="F209" s="78">
         <v>42550.798055555555</v>
       </c>
-      <c r="G209" s="85">
-        <v>1</v>
-      </c>
-      <c r="H209" s="84" t="s">
+      <c r="G209" s="79">
+        <v>1</v>
+      </c>
+      <c r="H209" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="I209" s="84">
+      <c r="I209" s="78">
         <v>42551.252083333333</v>
       </c>
       <c r="J209" s="51">
@@ -20750,47 +20536,47 @@
     <mergeCell ref="I3:J3"/>
   </mergeCells>
   <conditionalFormatting sqref="W11:W12 W13:X1048576">
-    <cfRule type="cellIs" dxfId="19" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="75" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X13:X1048576">
-    <cfRule type="cellIs" dxfId="18" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="58" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X12:X1048576">
-    <cfRule type="cellIs" dxfId="17" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="55" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:S14 A13:J13 L13:S13 K155:M209 A15:M154 N15:S209">
-    <cfRule type="expression" dxfId="16" priority="51">
+    <cfRule type="expression" dxfId="12" priority="51">
       <formula>$O13&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:S14 A13:J13 L13:S13 K155:M209 A15:M154 N15:S209">
-    <cfRule type="expression" dxfId="15" priority="50">
+    <cfRule type="expression" dxfId="11" priority="50">
       <formula>$P13&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="expression" dxfId="14" priority="6">
+    <cfRule type="expression" dxfId="10" priority="6">
       <formula>$O13&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="expression" dxfId="13" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>$P13&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A156:J156">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula>$O156&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A156:J156">
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>$P156&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20848,8 +20634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q116"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20904,22 +20690,22 @@
       <c r="P4" s="44"/>
     </row>
     <row r="5" spans="1:17" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="77" t="str">
+      <c r="A5" s="104" t="str">
         <f>"Eagle P3 Braking Events - "&amp;TEXT(Variables!$A$2,"YYYY-mm-dd")</f>
         <v>Eagle P3 Braking Events - 2016-06-29</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="77"/>
+      <c r="B5" s="104"/>
+      <c r="C5" s="104"/>
+      <c r="D5" s="104"/>
+      <c r="E5" s="104"/>
+      <c r="F5" s="104"/>
+      <c r="G5" s="104"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="104"/>
+      <c r="J5" s="104"/>
+      <c r="K5" s="104"/>
+      <c r="L5" s="104"/>
+      <c r="M5" s="104"/>
       <c r="N5" s="17"/>
       <c r="P5" s="42"/>
     </row>
@@ -21019,7 +20805,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 04:38:41-0600',mode:absolute,to:'2016-06-29 05:23:02-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4032%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q7" s="9" t="str">
-        <f>MID(B7,13,4)</f>
+        <f t="shared" ref="Q7:Q38" si="0">MID(B7,13,4)</f>
         <v>4032</v>
       </c>
     </row>
@@ -21072,7 +20858,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 09:51:53-0600',mode:absolute,to:'2016-06-29 10:38:57-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4044%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q8" s="9" t="str">
-        <f>MID(B8,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4044</v>
       </c>
     </row>
@@ -21125,7 +20911,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 13:04:04-0600',mode:absolute,to:'2016-06-29 13:53:00-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4015%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q9" s="9" t="str">
-        <f>MID(B9,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4015</v>
       </c>
     </row>
@@ -21178,7 +20964,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 14:01:02-0600',mode:absolute,to:'2016-06-29 14:53:05-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4039%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q10" s="9" t="str">
-        <f>MID(B10,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4039</v>
       </c>
     </row>
@@ -21231,7 +21017,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 16:35:51-0600',mode:absolute,to:'2016-06-29 17:24:23-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4040%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q11" s="9" t="str">
-        <f>MID(B11,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4040</v>
       </c>
     </row>
@@ -21284,7 +21070,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 21:13:57-0600',mode:absolute,to:'2016-06-29 22:13:38-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4044%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q12" s="9" t="str">
-        <f>MID(B12,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4044</v>
       </c>
     </row>
@@ -21335,7 +21121,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 03:47:52-0600',mode:absolute,to:'2016-06-29 04:32:54-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4024%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q13" s="9" t="str">
-        <f>MID(B13,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4024</v>
       </c>
     </row>
@@ -21386,7 +21172,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 04:20:23-0600',mode:absolute,to:'2016-06-29 05:11:28-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4040%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q14" s="9" t="str">
-        <f>MID(B14,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4040</v>
       </c>
     </row>
@@ -21437,7 +21223,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 07:22:14-0600',mode:absolute,to:'2016-06-29 08:14:13-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4012%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q15" s="9" t="str">
-        <f>MID(B15,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4012</v>
       </c>
     </row>
@@ -21488,7 +21274,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 08:23:17-0600',mode:absolute,to:'2016-06-29 09:07:41-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4011%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q16" s="9" t="str">
-        <f>MID(B16,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4011</v>
       </c>
     </row>
@@ -21539,7 +21325,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 09:08:42-0600',mode:absolute,to:'2016-06-29 10:04:50-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4012%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q17" s="9" t="str">
-        <f>MID(B17,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4012</v>
       </c>
     </row>
@@ -21590,7 +21376,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 10:08:39-0600',mode:absolute,to:'2016-06-29 10:51:29-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4032%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q18" s="9" t="str">
-        <f>MID(B18,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4032</v>
       </c>
     </row>
@@ -21641,7 +21427,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 12:00:25-0600',mode:absolute,to:'2016-06-29 12:47:04-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4011%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q19" s="9" t="str">
-        <f>MID(B19,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4011</v>
       </c>
     </row>
@@ -21692,7 +21478,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 12:27:59-0600',mode:absolute,to:'2016-06-29 13:18:36-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4024%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q20" s="9" t="str">
-        <f>MID(B20,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4024</v>
       </c>
     </row>
@@ -21743,7 +21529,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 12:54:32-0600',mode:absolute,to:'2016-06-29 13:16:37-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4042%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q21" s="9" t="str">
-        <f>MID(B21,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4042</v>
       </c>
     </row>
@@ -21794,7 +21580,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 13:54:59-0600',mode:absolute,to:'2016-06-29 14:51:01-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4016%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q22" s="9" t="str">
-        <f>MID(B22,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4016</v>
       </c>
     </row>
@@ -21845,7 +21631,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 13:54:59-0600',mode:absolute,to:'2016-06-29 14:51:01-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4016%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q23" s="9" t="str">
-        <f>MID(B23,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4016</v>
       </c>
     </row>
@@ -21896,7 +21682,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 14:10:04-0600',mode:absolute,to:'2016-06-29 14:58:06-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4024%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q24" s="9" t="str">
-        <f>MID(B24,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4024</v>
       </c>
     </row>
@@ -21947,7 +21733,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 15:47:03-0600',mode:absolute,to:'2016-06-29 16:35:49-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4039%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q25" s="9" t="str">
-        <f>MID(B25,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4039</v>
       </c>
     </row>
@@ -21998,7 +21784,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 16:39:38-0600',mode:absolute,to:'2016-06-29 17:25:14-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4043%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q26" s="9" t="str">
-        <f>MID(B26,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4043</v>
       </c>
     </row>
@@ -22049,7 +21835,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 20:48:05-0600',mode:absolute,to:'2016-06-29 21:34:19-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4041%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q27" s="9" t="str">
-        <f>MID(B27,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4041</v>
       </c>
     </row>
@@ -22100,7 +21886,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 22:50:57-0600',mode:absolute,to:'2016-06-29 23:36:37-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4041%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q28" s="9" t="str">
-        <f>MID(B28,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4041</v>
       </c>
     </row>
@@ -22151,7 +21937,7 @@
         <v>0</v>
       </c>
       <c r="Q29" s="9" t="str">
-        <f>MID(B29,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4018</v>
       </c>
     </row>
@@ -22202,7 +21988,7 @@
         <v>0</v>
       </c>
       <c r="Q30" s="9" t="str">
-        <f>MID(B30,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4017</v>
       </c>
     </row>
@@ -22253,7 +22039,7 @@
         <v>0</v>
       </c>
       <c r="Q31" s="9" t="str">
-        <f>MID(B31,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4018</v>
       </c>
     </row>
@@ -22305,7 +22091,7 @@
         <v>0</v>
       </c>
       <c r="Q32" s="9" t="str">
-        <f>MID(B32,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4018</v>
       </c>
     </row>
@@ -22357,7 +22143,7 @@
         <v>0</v>
       </c>
       <c r="Q33" s="9" t="str">
-        <f>MID(B33,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4018</v>
       </c>
     </row>
@@ -22409,7 +22195,7 @@
         <v>0</v>
       </c>
       <c r="Q34" s="9" t="str">
-        <f>MID(B34,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4018</v>
       </c>
     </row>
@@ -22461,7 +22247,7 @@
         <v>0</v>
       </c>
       <c r="Q35" s="9" t="str">
-        <f>MID(B35,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4017</v>
       </c>
     </row>
@@ -22513,7 +22299,7 @@
         <v>0</v>
       </c>
       <c r="Q36" s="9" t="str">
-        <f>MID(B36,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4029</v>
       </c>
     </row>
@@ -22567,7 +22353,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 05:03:36-0600',mode:absolute,to:'2016-06-29 05:51:37-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4013%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q37" s="9" t="str">
-        <f>MID(B37,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4013</v>
       </c>
     </row>
@@ -22621,7 +22407,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 07:39:21-0600',mode:absolute,to:'2016-06-29 08:10:37-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4031%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q38" s="9" t="str">
-        <f>MID(B38,13,4)</f>
+        <f t="shared" si="0"/>
         <v>4031</v>
       </c>
     </row>
@@ -22675,7 +22461,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 08:22:26-0600',mode:absolute,to:'2016-06-29 09:10:48-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4032%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q39" s="9" t="str">
-        <f>MID(B39,13,4)</f>
+        <f t="shared" ref="Q39:Q70" si="1">MID(B39,13,4)</f>
         <v>4032</v>
       </c>
     </row>
@@ -22729,7 +22515,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 09:23:17-0600',mode:absolute,to:'2016-06-29 10:18:31-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4015%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q40" s="9" t="str">
-        <f>MID(B40,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4015</v>
       </c>
     </row>
@@ -22783,7 +22569,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 09:42:34-0600',mode:absolute,to:'2016-06-29 10:17:42-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4040%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q41" s="9" t="str">
-        <f>MID(B41,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4040</v>
       </c>
     </row>
@@ -22837,7 +22623,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 13:04:04-0600',mode:absolute,to:'2016-06-29 13:53:00-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4015%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q42" s="9" t="str">
-        <f>MID(B42,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4015</v>
       </c>
     </row>
@@ -22891,7 +22677,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 14:01:02-0600',mode:absolute,to:'2016-06-29 14:53:05-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4039%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q43" s="9" t="str">
-        <f>MID(B43,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4039</v>
       </c>
     </row>
@@ -22945,7 +22731,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 16:22:29-0600',mode:absolute,to:'2016-06-29 17:14:08-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4012%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q44" s="9" t="str">
-        <f>MID(B44,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4012</v>
       </c>
     </row>
@@ -22999,7 +22785,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 18:06:54-0600',mode:absolute,to:'2016-06-29 18:57:13-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4012%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q45" s="9" t="str">
-        <f>MID(B45,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4012</v>
       </c>
     </row>
@@ -23053,7 +22839,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 23:55:53-0600',mode:absolute,to:'2016-06-30 00:18:54-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4042%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q46" s="9" t="str">
-        <f>MID(B46,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4042</v>
       </c>
     </row>
@@ -23107,7 +22893,7 @@
         <v>0</v>
       </c>
       <c r="Q47" s="9" t="str">
-        <f>MID(B47,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4030</v>
       </c>
     </row>
@@ -23161,7 +22947,7 @@
         <v>0</v>
       </c>
       <c r="Q48" s="9" t="str">
-        <f>MID(B48,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4017</v>
       </c>
     </row>
@@ -23215,7 +23001,7 @@
         <v>0</v>
       </c>
       <c r="Q49" s="9" t="str">
-        <f>MID(B49,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4017</v>
       </c>
     </row>
@@ -23269,7 +23055,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 08:05:56-0600',mode:absolute,to:'2016-06-29 08:51:07-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4023%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q50" s="9" t="str">
-        <f>MID(B50,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4023</v>
       </c>
     </row>
@@ -23322,7 +23108,7 @@
         <v>0</v>
       </c>
       <c r="Q51" s="9" t="str">
-        <f>MID(B51,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4018</v>
       </c>
     </row>
@@ -23374,7 +23160,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 04:50:57-0600',mode:absolute,to:'2016-06-29 05:40:40-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4011%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q52" s="9" t="str">
-        <f>MID(B52,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4011</v>
       </c>
     </row>
@@ -23426,7 +23212,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 06:51:43-0600',mode:absolute,to:'2016-06-29 07:36:36-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4016%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q53" s="9" t="str">
-        <f>MID(B53,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4016</v>
       </c>
     </row>
@@ -23478,7 +23264,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 08:05:56-0600',mode:absolute,to:'2016-06-29 08:51:07-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4023%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q54" s="9" t="str">
-        <f>MID(B54,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4023</v>
       </c>
     </row>
@@ -23530,7 +23316,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 07:39:21-0600',mode:absolute,to:'2016-06-29 08:10:37-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4031%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q55" s="9" t="str">
-        <f>MID(B55,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4031</v>
       </c>
     </row>
@@ -23582,7 +23368,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 10:20:06-0600',mode:absolute,to:'2016-06-29 11:07:46-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4016%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q56" s="9" t="str">
-        <f>MID(B56,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4016</v>
       </c>
     </row>
@@ -23634,7 +23420,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 11:35:12-0600',mode:absolute,to:'2016-06-29 12:28:04-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4023%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q57" s="9" t="str">
-        <f>MID(B57,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4023</v>
       </c>
     </row>
@@ -23686,7 +23472,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 11:09:50-0600',mode:absolute,to:'2016-06-29 12:01:24-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4042%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q58" s="9" t="str">
-        <f>MID(B58,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4042</v>
       </c>
     </row>
@@ -23738,7 +23524,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 11:09:50-0600',mode:absolute,to:'2016-06-29 12:01:24-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4042%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q59" s="9" t="str">
-        <f>MID(B59,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4042</v>
       </c>
     </row>
@@ -23790,7 +23576,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 12:52:20-0600',mode:absolute,to:'2016-06-29 13:41:21-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4012%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q60" s="9" t="str">
-        <f>MID(B60,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4012</v>
       </c>
     </row>
@@ -23842,7 +23628,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 13:04:04-0600',mode:absolute,to:'2016-06-29 13:53:00-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4015%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q61" s="9" t="str">
-        <f>MID(B61,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4015</v>
       </c>
     </row>
@@ -23894,7 +23680,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 15:47:03-0600',mode:absolute,to:'2016-06-29 16:35:49-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4039%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q62" s="9" t="str">
-        <f>MID(B62,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4039</v>
       </c>
     </row>
@@ -23946,7 +23732,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 15:47:03-0600',mode:absolute,to:'2016-06-29 16:35:49-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4039%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q63" s="9" t="str">
-        <f>MID(B63,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4039</v>
       </c>
     </row>
@@ -23998,7 +23784,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 16:22:29-0600',mode:absolute,to:'2016-06-29 17:14:08-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4012%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q64" s="9" t="str">
-        <f>MID(B64,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4012</v>
       </c>
     </row>
@@ -24050,7 +23836,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 16:22:29-0600',mode:absolute,to:'2016-06-29 17:14:08-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4012%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q65" s="9" t="str">
-        <f>MID(B65,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4012</v>
       </c>
     </row>
@@ -24102,7 +23888,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 16:26:33-0600',mode:absolute,to:'2016-06-29 17:11:19-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4042%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q66" s="9" t="str">
-        <f>MID(B66,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4042</v>
       </c>
     </row>
@@ -24154,7 +23940,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 18:06:54-0600',mode:absolute,to:'2016-06-29 18:57:13-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4012%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q67" s="9" t="str">
-        <f>MID(B67,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4012</v>
       </c>
     </row>
@@ -24206,7 +23992,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 17:26:12-0600',mode:absolute,to:'2016-06-29 18:09:30-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4044%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q68" s="9" t="str">
-        <f>MID(B68,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4044</v>
       </c>
     </row>
@@ -24258,7 +24044,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 20:18:11-0600',mode:absolute,to:'2016-06-29 21:06:23-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4043%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q69" s="9" t="str">
-        <f>MID(B69,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4043</v>
       </c>
     </row>
@@ -24310,7 +24096,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 21:20:39-0600',mode:absolute,to:'2016-06-29 22:08:24-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4039%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q70" s="9" t="str">
-        <f>MID(B70,13,4)</f>
+        <f t="shared" si="1"/>
         <v>4039</v>
       </c>
     </row>
@@ -24362,7 +24148,7 @@
         <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-06-29 22:50:57-0600',mode:absolute,to:'2016-06-29 23:36:37-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4041%22')),sort:!(Time,asc))</v>
       </c>
       <c r="Q71" s="9" t="str">
-        <f>MID(B71,13,4)</f>
+        <f t="shared" ref="Q71:Q85" si="2">MID(B71,13,4)</f>
         <v>4041</v>
       </c>
     </row>
@@ -24414,7 +24200,7 @@
         <v>0</v>
       </c>
       <c r="Q72" s="9" t="str">
-        <f>MID(B72,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4017</v>
       </c>
     </row>
@@ -24466,7 +24252,7 @@
         <v>0</v>
       </c>
       <c r="Q73" s="9" t="str">
-        <f>MID(B73,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4029</v>
       </c>
     </row>
@@ -24518,7 +24304,7 @@
         <v>0</v>
       </c>
       <c r="Q74" s="9" t="str">
-        <f>MID(B74,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4018</v>
       </c>
     </row>
@@ -24570,7 +24356,7 @@
         <v>0</v>
       </c>
       <c r="Q75" s="9" t="str">
-        <f>MID(B75,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4017</v>
       </c>
     </row>
@@ -24621,7 +24407,7 @@
         <v>0</v>
       </c>
       <c r="Q76" s="9" t="str">
-        <f>MID(B76,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4018</v>
       </c>
     </row>
@@ -24672,7 +24458,7 @@
         <v>0</v>
       </c>
       <c r="Q77" s="9" t="str">
-        <f>MID(B77,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4018</v>
       </c>
     </row>
@@ -24723,7 +24509,7 @@
         <v>0</v>
       </c>
       <c r="Q78" s="9" t="str">
-        <f>MID(B78,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4018</v>
       </c>
     </row>
@@ -24774,7 +24560,7 @@
         <v>0</v>
       </c>
       <c r="Q79" s="9" t="str">
-        <f>MID(B79,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4030</v>
       </c>
     </row>
@@ -24825,7 +24611,7 @@
         <v>0</v>
       </c>
       <c r="Q80" s="9" t="str">
-        <f>MID(B80,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4018</v>
       </c>
     </row>
@@ -24876,7 +24662,7 @@
         <v>0</v>
       </c>
       <c r="Q81" s="9" t="str">
-        <f>MID(B81,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4018</v>
       </c>
     </row>
@@ -24927,7 +24713,7 @@
         <v>0</v>
       </c>
       <c r="Q82" s="9" t="str">
-        <f>MID(B82,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4030</v>
       </c>
     </row>
@@ -24978,7 +24764,7 @@
         <v>0</v>
       </c>
       <c r="Q83" s="9" t="str">
-        <f>MID(B83,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4018</v>
       </c>
     </row>
@@ -25029,7 +24815,7 @@
         <v>0</v>
       </c>
       <c r="Q84" s="9" t="str">
-        <f>MID(B84,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4018</v>
       </c>
     </row>
@@ -25080,7 +24866,7 @@
         <v>0</v>
       </c>
       <c r="Q85" s="9" t="str">
-        <f>MID(B85,13,4)</f>
+        <f t="shared" si="2"/>
         <v>4018</v>
       </c>
     </row>
@@ -25544,22 +25330,22 @@
     <mergeCell ref="A5:M5"/>
   </mergeCells>
   <conditionalFormatting sqref="P6 M6:N6 M7:M1048576">
-    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="12" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M52:N69 L52:L116 A52:K69 A7:N51">
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>$M7="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M3">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M51">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25588,14 +25374,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="str">
+      <c r="A1" s="105" t="str">
         <f>"Trips that did not appear in PTC Data "&amp;TEXT(Variables!$A$2,"YYYY-mm-dd")</f>
         <v>Trips that did not appear in PTC Data 2016-06-29</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
     </row>
     <row r="2" spans="1:10" s="41" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">

</xml_diff>